<commit_message>
1.Fix the 7805 unknown pin problem, the pin number should match footprint
</commit_message>
<xml_diff>
--- a/36V single OP version/Project Outputs for Single motor monitoring Beta/Single motor monitoring Beta.xlsx
+++ b/36V single OP version/Project Outputs for Single motor monitoring Beta/Single motor monitoring Beta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kzhou\Desktop\RF projects\RF 36V motor controller\PCB-project\36V single OP version\Project Outputs for Single motor monitoring Beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2B456EA-B2DD-45A4-AC04-4AC95CDE8087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0F8A28-F66A-4D04-BEC1-4A7BF4A3C586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{2A7F716F-0213-4268-8EF1-781DCC303BB8}"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{2A7F716F-0213-4268-8EF1-781DCC303BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Single motor monitoring Beta" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
   <si>
     <t>Comment</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>LM358AM</t>
+  </si>
+  <si>
+    <t>Shopping car</t>
   </si>
 </sst>
 </file>
@@ -776,16 +779,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -804,8 +810,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -825,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -845,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -865,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -885,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -905,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -925,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -945,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -965,7 +974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -985,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
@@ -1045,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
@@ -1065,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
@@ -1085,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>